<commit_message>
upravena logika funkce "přidat kod"
</commit_message>
<xml_diff>
--- a/12052023.xlsx
+++ b/12052023.xlsx
@@ -1172,7 +1172,11 @@
           <t>Musa sikkimensis x balbisiana</t>
         </is>
       </c>
-      <c r="D13" s="9" t="n"/>
+      <c r="D13" s="9" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E13" s="9" t="n"/>
       <c r="F13" s="6" t="n"/>
     </row>
@@ -1511,7 +1515,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D15" s="11" t="n"/>
+      <c r="D15" s="11" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E15" s="11" t="n"/>
       <c r="F15" s="6" t="n"/>
     </row>
@@ -1523,7 +1531,11 @@
           <t>Musa sikkimensis x balbisiana</t>
         </is>
       </c>
-      <c r="D16" s="11" t="n"/>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E16" s="11" t="n"/>
       <c r="F16" s="6" t="n"/>
     </row>
@@ -1830,8 +1842,16 @@
           <t>Dasylirion wheeleri</t>
         </is>
       </c>
-      <c r="D14" s="23" t="n"/>
-      <c r="E14" s="9" t="n"/>
+      <c r="D14" s="23" t="inlineStr">
+        <is>
+          <t>adasdasd</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F14" s="6" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="58">
@@ -1842,8 +1862,16 @@
           <t>Agave havardiana</t>
         </is>
       </c>
-      <c r="D15" s="41" t="n"/>
-      <c r="E15" s="9" t="n"/>
+      <c r="D15" s="41" t="inlineStr">
+        <is>
+          <t>22-Ro976</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F15" s="6" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="58">
@@ -1854,8 +1882,16 @@
           <t>Agave parryi var. Parryi</t>
         </is>
       </c>
-      <c r="D16" s="41" t="n"/>
-      <c r="E16" s="9" t="n"/>
+      <c r="D16" s="41" t="inlineStr">
+        <is>
+          <t>vyližete mi prdel prosim</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F16" s="6" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="58">
@@ -2416,7 +2452,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D14" s="24" t="n"/>
+      <c r="D14" s="24" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E14" s="11" t="n"/>
       <c r="F14" s="6" t="n"/>
     </row>
@@ -2755,8 +2795,16 @@
           <t>Monstera dubia</t>
         </is>
       </c>
-      <c r="D16" s="41" t="n"/>
-      <c r="E16" s="9" t="n"/>
+      <c r="D16" s="41" t="inlineStr">
+        <is>
+          <t>miluju tě olinko</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F16" s="6" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="58">
@@ -2767,8 +2815,16 @@
           <t>Epipremnum pinnatum "Blue form"</t>
         </is>
       </c>
-      <c r="D17" s="24" t="n"/>
-      <c r="E17" s="9" t="n"/>
+      <c r="D17" s="24" t="inlineStr">
+        <is>
+          <t>kokot</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F17" s="6" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="58">
@@ -2779,8 +2835,16 @@
           <t>Epipremnum "happy leaf"</t>
         </is>
       </c>
-      <c r="D18" s="24" t="n"/>
-      <c r="E18" s="9" t="n"/>
+      <c r="D18" s="24" t="inlineStr">
+        <is>
+          <t>tudum</t>
+        </is>
+      </c>
+      <c r="E18" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F18" s="6" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="58">
@@ -2791,8 +2855,16 @@
           <t>Epipremnum "Marble quee</t>
         </is>
       </c>
-      <c r="D19" s="24" t="n"/>
-      <c r="E19" s="9" t="n"/>
+      <c r="D19" s="24" t="inlineStr">
+        <is>
+          <t>lolo</t>
+        </is>
+      </c>
+      <c r="E19" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F19" s="6" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="58">
@@ -2803,8 +2875,16 @@
           <t>Epipremnum "neon</t>
         </is>
       </c>
-      <c r="D20" s="24" t="n"/>
-      <c r="E20" s="9" t="n"/>
+      <c r="D20" s="24" t="inlineStr">
+        <is>
+          <t>trololo</t>
+        </is>
+      </c>
+      <c r="E20" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F20" s="6" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="58">
@@ -3706,7 +3786,11 @@
           <t xml:space="preserve">Passiflora x colvillii </t>
         </is>
       </c>
-      <c r="D14" s="38" t="n"/>
+      <c r="D14" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E14" s="38" t="n"/>
       <c r="F14" s="6" t="n"/>
     </row>
@@ -3718,8 +3802,16 @@
           <t>Marhaník granátový "Acco"</t>
         </is>
       </c>
-      <c r="D15" s="38" t="n"/>
-      <c r="E15" s="38" t="n"/>
+      <c r="D15" s="38" t="inlineStr">
+        <is>
+          <t>nigga</t>
+        </is>
+      </c>
+      <c r="E15" s="38" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F15" s="6" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="58">
@@ -3762,8 +3854,16 @@
           <t>Ugni molinae "Elite"</t>
         </is>
       </c>
-      <c r="D18" s="38" t="n"/>
-      <c r="E18" s="38" t="n"/>
+      <c r="D18" s="38" t="inlineStr">
+        <is>
+          <t>nuggo</t>
+        </is>
+      </c>
+      <c r="E18" s="38" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F18" s="6" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="58">
@@ -4607,7 +4707,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D13" s="38" t="n"/>
+      <c r="D13" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E13" s="38" t="n"/>
       <c r="F13" s="6" t="n"/>
     </row>
@@ -4968,7 +5072,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D17" s="38" t="n"/>
+      <c r="D17" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E17" s="38" t="n"/>
       <c r="F17" s="6" t="n"/>
     </row>
@@ -5759,8 +5867,16 @@
           <t xml:space="preserve">Pinus nigra </t>
         </is>
       </c>
-      <c r="D14" s="38" t="n"/>
-      <c r="E14" s="38" t="n"/>
+      <c r="D14" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro234</t>
+        </is>
+      </c>
+      <c r="E14" s="38" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F14" s="6" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="58">
@@ -6510,7 +6626,11 @@
           <t>Musa sikkimensis x balbisiana "Dajiao"</t>
         </is>
       </c>
-      <c r="D17" s="38" t="n"/>
+      <c r="D17" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E17" s="38" t="n"/>
       <c r="F17" s="6" t="n"/>
     </row>
@@ -8490,7 +8610,11 @@
           <t>Musa sikkimensis x balbisiana "Dajiao"</t>
         </is>
       </c>
-      <c r="D13" s="38" t="n"/>
+      <c r="D13" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E13" s="38" t="n"/>
       <c r="F13" s="6" t="n"/>
     </row>
@@ -8803,7 +8927,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D14" s="38" t="n"/>
+      <c r="D14" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E14" s="38" t="n"/>
       <c r="F14" s="6" t="n"/>
     </row>
@@ -9421,7 +9549,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D14" s="38" t="n"/>
+      <c r="D14" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E14" s="38" t="n"/>
       <c r="F14" s="6" t="n"/>
     </row>
@@ -9593,7 +9725,11 @@
           <t>Musa sikkimensis x balbisiana "Dajiao"</t>
         </is>
       </c>
-      <c r="D25" s="13" t="n"/>
+      <c r="D25" s="13" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E25" s="38" t="n"/>
       <c r="F25" s="6" t="n"/>
     </row>
@@ -10934,7 +11070,11 @@
           <t>Passiflora x colvill</t>
         </is>
       </c>
-      <c r="D15" s="38" t="n"/>
+      <c r="D15" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E15" s="38" t="n"/>
       <c r="F15" s="6" t="n"/>
     </row>
@@ -11467,7 +11607,11 @@
           <t xml:space="preserve">Passiflora x colvillii </t>
         </is>
       </c>
-      <c r="D30" s="38" t="n"/>
+      <c r="D30" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E30" s="38" t="n"/>
       <c r="F30" s="6" t="n"/>
     </row>
@@ -14673,7 +14817,11 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D17" s="38" t="n"/>
+      <c r="D17" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E17" s="38" t="n"/>
       <c r="F17" s="6" t="n"/>
     </row>
@@ -14717,7 +14865,11 @@
           <t>Musa sikkimensis x balbisiana</t>
         </is>
       </c>
-      <c r="D20" s="38" t="n"/>
+      <c r="D20" s="38" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
       <c r="E20" s="38" t="n"/>
       <c r="F20" s="6" t="n"/>
     </row>
@@ -16429,8 +16581,16 @@
           <t>Passiflora x colvillii</t>
         </is>
       </c>
-      <c r="D17" s="42" t="n"/>
-      <c r="E17" s="24" t="n"/>
+      <c r="D17" s="42" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
+      <c r="E17" s="24" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F17" s="6" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="58">
@@ -16696,8 +16856,16 @@
           <t>Musa sikkimensis x balbisiana</t>
         </is>
       </c>
-      <c r="D14" s="10" t="n"/>
-      <c r="E14" s="9" t="n"/>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>22-Ro1337</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F14" s="6" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="58">
@@ -16708,8 +16876,16 @@
           <t>Musa sikkimensis Red Tiger</t>
         </is>
       </c>
-      <c r="D15" s="46" t="n"/>
-      <c r="E15" s="9" t="n"/>
+      <c r="D15" s="46" t="inlineStr">
+        <is>
+          <t>22-Rk479</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F15" s="6" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="58">
@@ -17326,8 +17502,16 @@
           <t>Paeonia suffruticosa</t>
         </is>
       </c>
-      <c r="D15" s="41" t="n"/>
-      <c r="E15" s="44" t="n"/>
+      <c r="D15" s="41" t="inlineStr">
+        <is>
+          <t>vilimte si</t>
+        </is>
+      </c>
+      <c r="E15" s="44" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
       <c r="F15" s="6" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="58">
@@ -17338,7 +17522,11 @@
           <t xml:space="preserve">Passiflora x colvillii </t>
         </is>
       </c>
-      <c r="D16" s="42" t="n"/>
+      <c r="D16" s="42" t="inlineStr">
+        <is>
+          <t>22-Ro2</t>
+        </is>
+      </c>
       <c r="E16" s="44" t="n"/>
       <c r="F16" s="6" t="n"/>
     </row>

</xml_diff>